<commit_message>
- adjusted code in several places to merge with development branch
</commit_message>
<xml_diff>
--- a/data_processed/Further_Lists/data_CZ_2.xlsx
+++ b/data_processed/Further_Lists/data_CZ_2.xlsx
@@ -11,7 +11,7 @@
     <sheet name="source" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">pp_list_CZ2!$A$1:$O$74</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">pp_list_CZ2!$A$1:$P$74</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -746,7 +746,7 @@
   <dimension ref="A1:R74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,8 +763,8 @@
     <col min="12" max="12" width="14.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.7109375" customWidth="1"/>
+    <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -812,10 +812,10 @@
         <v>12</v>
       </c>
       <c r="O1" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>117</v>
       </c>
       <c r="Q1" s="3" t="s">
         <v>115</v>
@@ -844,6 +844,7 @@
       <c r="N2" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O2" s="3"/>
       <c r="Q2">
         <v>49.232349999999997</v>
       </c>
@@ -871,6 +872,7 @@
       <c r="N3" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O3" s="3"/>
       <c r="Q3">
         <v>49.218069999999997</v>
       </c>
@@ -898,6 +900,7 @@
       <c r="N4" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O4" s="3"/>
       <c r="Q4">
         <v>49.218069999999997</v>
       </c>
@@ -925,6 +928,7 @@
       <c r="N5" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O5" s="3"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
@@ -946,6 +950,7 @@
       <c r="N6" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O6" s="3"/>
       <c r="Q6">
         <v>49.191879999999998</v>
       </c>
@@ -973,6 +978,7 @@
       <c r="N7" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O7" s="3"/>
       <c r="Q7">
         <v>49.191879999999998</v>
       </c>
@@ -1000,6 +1006,7 @@
       <c r="N8" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O8" s="3"/>
       <c r="Q8">
         <v>49.191879999999998</v>
       </c>
@@ -1027,6 +1034,7 @@
       <c r="N9" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O9" s="3"/>
       <c r="Q9">
         <v>50.07743</v>
       </c>
@@ -1062,6 +1070,7 @@
       <c r="N10" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O10" s="3"/>
       <c r="Q10">
         <v>50.573239999999998</v>
       </c>
@@ -1089,6 +1098,7 @@
       <c r="N11" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O11" s="3"/>
       <c r="Q11">
         <v>49.181429999999999</v>
       </c>
@@ -1116,6 +1126,7 @@
       <c r="N12" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O12" s="3"/>
       <c r="Q12">
         <v>49.181429999999999</v>
       </c>
@@ -1146,6 +1157,7 @@
       <c r="N13" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O13" s="3"/>
       <c r="Q13">
         <v>48.84722</v>
       </c>
@@ -1173,6 +1185,7 @@
       <c r="N14" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O14" s="3"/>
       <c r="Q14">
         <v>49.79121</v>
       </c>
@@ -1200,6 +1213,7 @@
       <c r="N15" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O15" s="3"/>
       <c r="Q15">
         <v>50.207079999999998</v>
       </c>
@@ -1227,6 +1241,7 @@
       <c r="N16" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O16" s="3"/>
       <c r="Q16">
         <v>50.207079999999998</v>
       </c>
@@ -1254,6 +1269,7 @@
       <c r="N17" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O17" s="3"/>
       <c r="Q17">
         <v>50.207079999999998</v>
       </c>
@@ -1281,6 +1297,7 @@
       <c r="N18" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O18" s="3"/>
       <c r="Q18">
         <v>49.633650000000003</v>
       </c>
@@ -1308,6 +1325,7 @@
       <c r="N19" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O19" s="3"/>
       <c r="Q19">
         <v>49.633650000000003</v>
       </c>
@@ -1335,6 +1353,7 @@
       <c r="N20" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O20" s="3"/>
       <c r="Q20">
         <v>49.633650000000003</v>
       </c>
@@ -1362,6 +1381,7 @@
       <c r="N21" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O21" s="3"/>
       <c r="Q21">
         <v>49.633650000000003</v>
       </c>
@@ -1397,6 +1417,7 @@
       <c r="N22" s="3" t="s">
         <v>104</v>
       </c>
+      <c r="O22" s="3"/>
       <c r="Q22">
         <v>50.153669999999998</v>
       </c>
@@ -1426,6 +1447,7 @@
       <c r="N23" s="3" t="s">
         <v>104</v>
       </c>
+      <c r="O23" s="3"/>
       <c r="Q23">
         <v>50.153669999999998</v>
       </c>
@@ -1453,6 +1475,7 @@
       <c r="N24" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O24" s="3"/>
       <c r="Q24" s="6">
         <v>49.240900000000003</v>
       </c>
@@ -1480,6 +1503,7 @@
       <c r="N25" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O25" s="3"/>
       <c r="Q25" s="6">
         <v>49.240900000000003</v>
       </c>
@@ -1507,6 +1531,7 @@
       <c r="N26" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O26" s="3"/>
       <c r="Q26" s="6">
         <v>49.240900000000003</v>
       </c>
@@ -1534,6 +1559,7 @@
       <c r="N27" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O27" s="3"/>
       <c r="Q27" s="6">
         <v>50.45729</v>
       </c>
@@ -1561,6 +1587,7 @@
       <c r="N28" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O28" s="3"/>
       <c r="Q28" s="6">
         <v>50.45729</v>
       </c>
@@ -1591,7 +1618,8 @@
       <c r="N29" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="O29" t="s">
+      <c r="O29" s="3"/>
+      <c r="P29" t="s">
         <v>85</v>
       </c>
       <c r="Q29" s="6">
@@ -1624,7 +1652,8 @@
       <c r="N30" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="O30" t="s">
+      <c r="O30" s="3"/>
+      <c r="P30" t="s">
         <v>85</v>
       </c>
       <c r="Q30" s="6">
@@ -1654,6 +1683,7 @@
       <c r="N31" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O31" s="3"/>
       <c r="Q31" s="6">
         <v>48.633330000000001</v>
       </c>
@@ -1683,7 +1713,8 @@
       <c r="N32" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="O32" t="s">
+      <c r="O32" s="3"/>
+      <c r="P32" t="s">
         <v>113</v>
       </c>
       <c r="Q32">
@@ -1713,6 +1744,7 @@
       <c r="N33" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O33" s="3"/>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
@@ -1734,6 +1766,7 @@
       <c r="N34" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O34" s="3"/>
       <c r="Q34" s="6">
         <v>49.102370000000001</v>
       </c>
@@ -1761,6 +1794,7 @@
       <c r="N35" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O35" s="3"/>
       <c r="Q35" s="6">
         <v>49.102370000000001</v>
       </c>
@@ -1788,6 +1822,7 @@
       <c r="N36" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O36" s="3"/>
       <c r="Q36" s="6">
         <v>50.302100000000003</v>
       </c>
@@ -1815,6 +1850,7 @@
       <c r="N37" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O37" s="3"/>
       <c r="Q37" s="6">
         <v>50.302100000000003</v>
       </c>
@@ -1845,7 +1881,8 @@
       <c r="N38" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="O38" t="s">
+      <c r="O38" s="3"/>
+      <c r="P38" t="s">
         <v>90</v>
       </c>
       <c r="Q38">
@@ -1878,7 +1915,8 @@
       <c r="N39" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="O39" t="s">
+      <c r="O39" s="3"/>
+      <c r="P39" t="s">
         <v>90</v>
       </c>
       <c r="Q39">
@@ -1911,7 +1949,8 @@
       <c r="N40" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="O40" t="s">
+      <c r="O40" s="3"/>
+      <c r="P40" t="s">
         <v>90</v>
       </c>
       <c r="Q40">
@@ -1944,7 +1983,8 @@
       <c r="N41" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="O41" t="s">
+      <c r="O41" s="3"/>
+      <c r="P41" t="s">
         <v>90</v>
       </c>
       <c r="Q41">
@@ -1974,6 +2014,7 @@
       <c r="N42" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O42" s="3"/>
       <c r="Q42">
         <v>50.040579999999999</v>
       </c>
@@ -2001,6 +2042,7 @@
       <c r="N43" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O43" s="3"/>
       <c r="Q43">
         <v>50.075069999999997</v>
       </c>
@@ -2028,6 +2070,7 @@
       <c r="N44" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O44" s="3"/>
       <c r="Q44">
         <v>49.778190000000002</v>
       </c>
@@ -2055,6 +2098,7 @@
       <c r="N45" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O45" s="3"/>
       <c r="Q45">
         <v>49.778190000000002</v>
       </c>
@@ -2085,7 +2129,8 @@
       <c r="N46" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="O46" t="s">
+      <c r="O46" s="3"/>
+      <c r="P46" t="s">
         <v>92</v>
       </c>
       <c r="Q46">
@@ -2118,7 +2163,8 @@
       <c r="N47" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="O47" t="s">
+      <c r="O47" s="3"/>
+      <c r="P47" t="s">
         <v>92</v>
       </c>
       <c r="Q47">
@@ -2151,7 +2197,8 @@
       <c r="N48" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="O48" t="s">
+      <c r="O48" s="3"/>
+      <c r="P48" t="s">
         <v>92</v>
       </c>
       <c r="Q48">
@@ -2181,6 +2228,7 @@
       <c r="N49" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O49" s="3"/>
       <c r="Q49">
         <v>49.881149999999998</v>
       </c>
@@ -2208,6 +2256,7 @@
       <c r="N50" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O50" s="3"/>
       <c r="Q50">
         <v>50.25694</v>
       </c>
@@ -2235,6 +2284,7 @@
       <c r="N51" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O51" s="3"/>
       <c r="Q51">
         <v>50.043370000000003</v>
       </c>
@@ -2262,6 +2312,7 @@
       <c r="N52" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O52" s="3"/>
       <c r="Q52">
         <v>50.043370000000003</v>
       </c>
@@ -2289,6 +2340,7 @@
       <c r="N53" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O53" s="3"/>
       <c r="Q53">
         <v>50.043370000000003</v>
       </c>
@@ -2316,6 +2368,7 @@
       <c r="N54" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O54" s="3"/>
       <c r="Q54">
         <v>50.043370000000003</v>
       </c>
@@ -2346,7 +2399,8 @@
       <c r="N55" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="O55" t="s">
+      <c r="O55" s="3"/>
+      <c r="P55" t="s">
         <v>89</v>
       </c>
       <c r="Q55">
@@ -2379,7 +2433,8 @@
       <c r="N56" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="O56" t="s">
+      <c r="O56" s="3"/>
+      <c r="P56" t="s">
         <v>89</v>
       </c>
       <c r="Q56">
@@ -2412,7 +2467,8 @@
       <c r="N57" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="O57" t="s">
+      <c r="O57" s="3"/>
+      <c r="P57" t="s">
         <v>89</v>
       </c>
       <c r="Q57">
@@ -2442,6 +2498,7 @@
       <c r="N58" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O58" s="3"/>
     </row>
     <row r="59" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
@@ -2463,6 +2520,7 @@
       <c r="N59" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O59" s="3"/>
     </row>
     <row r="60" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
@@ -2484,6 +2542,7 @@
       <c r="N60" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O60" s="3"/>
       <c r="Q60">
         <v>49.135080000000002</v>
       </c>
@@ -2511,6 +2570,7 @@
       <c r="N61" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O61" s="3"/>
       <c r="Q61">
         <v>49.135080000000002</v>
       </c>
@@ -2538,6 +2598,7 @@
       <c r="N62" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O62" s="3"/>
       <c r="Q62">
         <v>49.84648</v>
       </c>
@@ -2565,6 +2626,7 @@
       <c r="N63" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O63" s="3"/>
       <c r="Q63">
         <v>49.84648</v>
       </c>
@@ -2595,6 +2657,7 @@
       <c r="N64" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O64" s="3"/>
       <c r="Q64">
         <v>49.84187</v>
       </c>
@@ -2621,6 +2684,7 @@
       <c r="N65" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O65" s="3"/>
       <c r="Q65">
         <v>50.638629999999999</v>
       </c>
@@ -2650,7 +2714,8 @@
       <c r="N66" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="O66" t="s">
+      <c r="O66" s="3"/>
+      <c r="P66" t="s">
         <v>93</v>
       </c>
       <c r="Q66">
@@ -2687,6 +2752,7 @@
       <c r="N67" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O67" s="3"/>
       <c r="Q67">
         <v>50.64584</v>
       </c>
@@ -2714,6 +2780,7 @@
       <c r="N68" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O68" s="3"/>
       <c r="Q68">
         <v>49.938160000000003</v>
       </c>
@@ -2741,6 +2808,7 @@
       <c r="N69" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O69" s="3"/>
       <c r="Q69">
         <v>49.938160000000003</v>
       </c>
@@ -2768,6 +2836,7 @@
       <c r="N70" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O70" s="3"/>
       <c r="Q70" s="6">
         <v>49.105699999999999</v>
       </c>
@@ -2795,6 +2864,7 @@
       <c r="N71" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O71" s="3"/>
       <c r="Q71" s="6">
         <v>49.105699999999999</v>
       </c>
@@ -2822,6 +2892,7 @@
       <c r="N72" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O72" s="3"/>
       <c r="Q72">
         <v>50.366390000000003</v>
       </c>
@@ -2849,6 +2920,7 @@
       <c r="N73" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="O73" s="3"/>
       <c r="Q73">
         <v>50.366390000000003</v>
       </c>
@@ -2884,6 +2956,7 @@
       <c r="N74" s="3" t="s">
         <v>104</v>
       </c>
+      <c r="O74" s="3"/>
       <c r="Q74">
         <v>49.226469999999999</v>
       </c>

</xml_diff>